<commit_message>
pulled the excel_filename out of all the functions to create a general variable
</commit_message>
<xml_diff>
--- a/homescraper/2024-02-19-house-analysis.xlsx
+++ b/homescraper/2024-02-19-house-analysis.xlsx
@@ -7,10 +7,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="1486-Olivewood-Ave-Lakewood-OH-44107" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="12929-Plover-St-Lakewood-OH-44107" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2040-Marlowe-Ave-Lakewood-OH-44107" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="11801-Franklin-Blvd-Lakewood-OH-44107" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="1356-W-64th-St-Cleveland-OH-44102" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="1276-W-67th-St-Cleveland-OH-44102" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="6911-Franklin-Blvd-Cleveland-OH-44102" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="1304-W-73rd-St-Cleveland-OH-44102" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -437,7 +437,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>1486 Olivewood Ave, Lakewood, OH 44107</t>
+          <t>1356 W 64th St, Cleveland, OH 44102</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -447,7 +447,7 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -457,7 +457,7 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
@@ -466,7 +466,7 @@
         </is>
       </c>
       <c r="H1" t="n">
-        <v>2408</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="3">
@@ -476,7 +476,7 @@
         </is>
       </c>
       <c r="B3" s="1" t="n">
-        <v>435000</v>
+        <v>459000</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -684,7 +684,7 @@
         </is>
       </c>
       <c r="B17" s="1" t="n">
-        <v>3498</v>
+        <v>6394</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -720,7 +720,7 @@
         </is>
       </c>
       <c r="B20" s="1" t="n">
-        <v>299.33</v>
+        <v>328.5</v>
       </c>
       <c r="C20">
         <f>B20</f>
@@ -738,7 +738,7 @@
         </is>
       </c>
       <c r="B21" s="1" t="n">
-        <v>217.5</v>
+        <v>229.5</v>
       </c>
       <c r="C21">
         <f>B21</f>
@@ -1138,7 +1138,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>12929 Plover St, Lakewood, OH 44107</t>
+          <t>1276 W 67th St, Cleveland, OH 44102</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -1148,7 +1148,7 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -1167,7 +1167,7 @@
         </is>
       </c>
       <c r="H1" t="n">
-        <v>2022</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="3">
@@ -1177,7 +1177,7 @@
         </is>
       </c>
       <c r="B3" s="1" t="n">
-        <v>265000</v>
+        <v>489000</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -1385,7 +1385,7 @@
         </is>
       </c>
       <c r="B17" s="1" t="n">
-        <v>2266</v>
+        <v>6882</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -1421,7 +1421,7 @@
         </is>
       </c>
       <c r="B20" s="1" t="n">
-        <v>187.33</v>
+        <v>515.58</v>
       </c>
       <c r="C20">
         <f>B20</f>
@@ -1439,7 +1439,7 @@
         </is>
       </c>
       <c r="B21" s="1" t="n">
-        <v>132.5</v>
+        <v>244.5</v>
       </c>
       <c r="C21">
         <f>B21</f>
@@ -1839,7 +1839,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>2040 Marlowe Ave, Lakewood, OH 44107</t>
+          <t>6911 Franklin Blvd, Cleveland, OH 44102</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -1859,7 +1859,7 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
@@ -1868,7 +1868,7 @@
         </is>
       </c>
       <c r="H1" t="n">
-        <v>4270</v>
+        <v>3976</v>
       </c>
     </row>
     <row r="3">
@@ -1878,7 +1878,7 @@
         </is>
       </c>
       <c r="B3" s="1" t="n">
-        <v>399500</v>
+        <v>525000</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -2086,7 +2086,7 @@
         </is>
       </c>
       <c r="B17" s="1" t="n">
-        <v>5478</v>
+        <v>3689</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -2122,7 +2122,7 @@
         </is>
       </c>
       <c r="B20" s="1" t="n">
-        <v>434.58</v>
+        <v>383.33</v>
       </c>
       <c r="C20">
         <f>B20</f>
@@ -2140,7 +2140,7 @@
         </is>
       </c>
       <c r="B21" s="1" t="n">
-        <v>199.75</v>
+        <v>262.5</v>
       </c>
       <c r="C21">
         <f>B21</f>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>11801 Franklin Blvd, Lakewood, OH 44107</t>
+          <t>1304 W 73rd St, Cleveland, OH 44102</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -2550,7 +2550,7 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -2569,7 +2569,7 @@
         </is>
       </c>
       <c r="H1" t="n">
-        <v>2086</v>
+        <v>2736</v>
       </c>
     </row>
     <row r="3">
@@ -2579,7 +2579,7 @@
         </is>
       </c>
       <c r="B3" s="1" t="n">
-        <v>289000</v>
+        <v>240000</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -2787,7 +2787,7 @@
         </is>
       </c>
       <c r="B17" s="1" t="n">
-        <v>2738</v>
+        <v>2420</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -2823,7 +2823,7 @@
         </is>
       </c>
       <c r="B20" s="1" t="n">
-        <v>251</v>
+        <v>212.5</v>
       </c>
       <c r="C20">
         <f>B20</f>
@@ -2841,7 +2841,7 @@
         </is>
       </c>
       <c r="B21" s="1" t="n">
-        <v>144.5</v>
+        <v>120</v>
       </c>
       <c r="C21">
         <f>B21</f>

</xml_diff>

<commit_message>
corrected formulas in 'house_excel_sheet_creator'
</commit_message>
<xml_diff>
--- a/homescraper/2024-02-19-house-analysis.xlsx
+++ b/homescraper/2024-02-19-house-analysis.xlsx
@@ -1062,19 +1062,19 @@
         <v/>
       </c>
       <c r="D33" s="1">
-        <f>D28*(1-B5)+sum(B32:C32)-E6-D30</f>
+        <f>D28*(1-0.08)+sum(B32:C32)-E6-D30</f>
         <v/>
       </c>
       <c r="E33" s="1">
-        <f>E28*(1-B5)+sum(B32:D32)-E6-E30</f>
+        <f>E28*(1-0.08)+sum(B32:D32)-E6-E30</f>
         <v/>
       </c>
       <c r="F33" s="1">
-        <f>F28*(1-B5)+sum(B32:E32)-E6-F30</f>
+        <f>F28*(1-0.08)+sum(B32:E32)-E6-F30</f>
         <v/>
       </c>
       <c r="G33" s="1">
-        <f>G28*(1-B5)+sum(B32:F32)-E6-G30</f>
+        <f>G28*(1-0.08)+sum(B32:F32)-E6-G30</f>
         <v/>
       </c>
       <c r="H33" s="1" t="n"/>
@@ -1763,19 +1763,19 @@
         <v/>
       </c>
       <c r="D33" s="1">
-        <f>D28*(1-B5)+sum(B32:C32)-E6-D30</f>
+        <f>D28*(1-0.08)+sum(B32:C32)-E6-D30</f>
         <v/>
       </c>
       <c r="E33" s="1">
-        <f>E28*(1-B5)+sum(B32:D32)-E6-E30</f>
+        <f>E28*(1-0.08)+sum(B32:D32)-E6-E30</f>
         <v/>
       </c>
       <c r="F33" s="1">
-        <f>F28*(1-B5)+sum(B32:E32)-E6-F30</f>
+        <f>F28*(1-0.08)+sum(B32:E32)-E6-F30</f>
         <v/>
       </c>
       <c r="G33" s="1">
-        <f>G28*(1-B5)+sum(B32:F32)-E6-G30</f>
+        <f>G28*(1-0.08)+sum(B32:F32)-E6-G30</f>
         <v/>
       </c>
       <c r="H33" s="1" t="n"/>
@@ -2464,19 +2464,19 @@
         <v/>
       </c>
       <c r="D33" s="1">
-        <f>D28*(1-B5)+sum(B32:C32)-E6-D30</f>
+        <f>D28*(1-0.08)+sum(B32:C32)-E6-D30</f>
         <v/>
       </c>
       <c r="E33" s="1">
-        <f>E28*(1-B5)+sum(B32:D32)-E6-E30</f>
+        <f>E28*(1-0.08)+sum(B32:D32)-E6-E30</f>
         <v/>
       </c>
       <c r="F33" s="1">
-        <f>F28*(1-B5)+sum(B32:E32)-E6-F30</f>
+        <f>F28*(1-0.08)+sum(B32:E32)-E6-F30</f>
         <v/>
       </c>
       <c r="G33" s="1">
-        <f>G28*(1-B5)+sum(B32:F32)-E6-G30</f>
+        <f>G28*(1-0.08)+sum(B32:F32)-E6-G30</f>
         <v/>
       </c>
       <c r="H33" s="1" t="n"/>
@@ -3165,19 +3165,19 @@
         <v/>
       </c>
       <c r="D33" s="1">
-        <f>D28*(1-B5)+sum(B32:C32)-E6-D30</f>
+        <f>D28*(1-0.08)+sum(B32:C32)-E6-D30</f>
         <v/>
       </c>
       <c r="E33" s="1">
-        <f>E28*(1-B5)+sum(B32:D32)-E6-E30</f>
+        <f>E28*(1-0.08)+sum(B32:D32)-E6-E30</f>
         <v/>
       </c>
       <c r="F33" s="1">
-        <f>F28*(1-B5)+sum(B32:E32)-E6-F30</f>
+        <f>F28*(1-0.08)+sum(B32:E32)-E6-F30</f>
         <v/>
       </c>
       <c r="G33" s="1">
-        <f>G28*(1-B5)+sum(B32:F32)-E6-G30</f>
+        <f>G28*(1-0.08)+sum(B32:F32)-E6-G30</f>
         <v/>
       </c>
       <c r="H33" s="1" t="n"/>

</xml_diff>